<commit_message>
compansation bitmiş haldedir. kablo tipi seçilecek. loadprofile.xlsx'e fazladan 1 tane leading pf li load eklenmiştir. çalışıyor denendi
</commit_message>
<xml_diff>
--- a/load_profile.xlsx
+++ b/load_profile.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6744" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6744" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Load1" sheetId="1" r:id="rId1"/>
     <sheet name="Load2" sheetId="2" r:id="rId2"/>
-    <sheet name="Load3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sayfa1" sheetId="4" r:id="rId3"/>
+    <sheet name="Load3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>Hour</t>
   </si>
@@ -671,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="A1:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,6 +959,296 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>75</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>75</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>75</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>50</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>75</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>100</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>125</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>125</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>100</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>75</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>

</xml_diff>